<commit_message>
Design Space updates (icons, videos, mechanisms)
</commit_message>
<xml_diff>
--- a/src/data/design_space.xlsx
+++ b/src/data/design_space.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spili\Documents\GitHub\Design-Space-Explorer\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2967F3E8-78AF-4215-855E-A330FD9A6B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8DB4A3-218F-4A0F-BC82-C05A979FE559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="17172" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dimensions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="361">
   <si>
     <t>dimension_id</t>
   </si>
@@ -140,9 +140,6 @@
     <t>spatial-attributes</t>
   </si>
   <si>
-    <t>Spatial Attirbutes</t>
-  </si>
-  <si>
     <t>#3f4adb</t>
   </si>
   <si>
@@ -650,9 +647,6 @@
     <t>"/Design-Space-Explorer/design_space_static/stretch.png"</t>
   </si>
   <si>
-    <t>"/Design-Space-Explorer/design_space_static/breaking.png"</t>
-  </si>
-  <si>
     <t>"/Design-Space-Explorer/design_space_static/camera2.png"</t>
   </si>
   <si>
@@ -1017,13 +1011,109 @@
   </si>
   <si>
     <t>ex-056</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/icons/shape.png"</t>
+  </si>
+  <si>
+    <t>Spatial Attributes</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/shatter.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/fold.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/shatter.gif"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/fold.gif"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/fluids.gif"</t>
+  </si>
+  <si>
+    <t>@daytogu</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/daytogu/</t>
+  </si>
+  <si>
+    <t>mechanism_creator</t>
+  </si>
+  <si>
+    <t>mechanism_creator_link</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/growth.gif"</t>
+  </si>
+  <si>
+    <t>@superdesigners.co</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/superdesigners.co/?g=5</t>
+  </si>
+  <si>
+    <t>@vincentschwenk</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/vincentschwenk/</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/deformable.gif"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/rigid.gif"</t>
+  </si>
+  <si>
+    <t>@benfryc_art</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/benfryc_art/?g=5</t>
+  </si>
+  <si>
+    <t>@kostsov</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/kostsov/?g=5</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/state_change.gif"</t>
+  </si>
+  <si>
+    <t>@marctudisco</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/marctudisco/</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/videos/infection.gif"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/fluids.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/state_change.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/deformable.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/rigid.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/infection.png"</t>
+  </si>
+  <si>
+    <t>"/Design-Space-Explorer/design_space_static/growth.png"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1056,6 +1146,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1079,10 +1177,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1113,8 +1212,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1419,7 +1522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1438,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
@@ -1467,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D2" t="s">
         <v>23</v>
@@ -1479,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1493,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>28</v>
@@ -1505,7 +1608,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -1519,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>31</v>
@@ -1545,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>32</v>
@@ -1571,19 +1674,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>330</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1591,13 +1694,13 @@
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1606,10 +1709,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>329</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1617,25 +1720,25 @@
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8">
         <v>3</v>
@@ -1643,25 +1746,25 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5">
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H9">
         <v>4</v>
@@ -1669,25 +1772,25 @@
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10">
         <v>5</v>
@@ -1695,25 +1798,25 @@
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H11">
         <v>6</v>
@@ -1721,23 +1824,23 @@
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12">
         <v>7</v>
@@ -1745,25 +1848,25 @@
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="5">
         <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1771,25 +1874,25 @@
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="5">
         <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -1797,25 +1900,25 @@
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B15" s="5">
         <v>3</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>241</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1823,23 +1926,23 @@
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B16" s="5">
         <v>3</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -1847,25 +1950,25 @@
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5">
         <v>3</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -1879,11 +1982,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1895,11 +1998,13 @@
     <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="6" max="6" width="46" customWidth="1"/>
     <col min="7" max="8" width="34" customWidth="1"/>
-    <col min="9" max="9" width="22" style="10" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="9" max="9" width="34" style="10" customWidth="1"/>
+    <col min="10" max="10" width="34" customWidth="1"/>
+    <col min="11" max="11" width="22" style="10" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1925,267 +2030,293 @@
         <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="J2" s="5">
+      <c r="I2" s="8"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="L2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="I3" s="8"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="L3" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="I4" s="8"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="I5" s="8"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="L5" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="J6" s="5">
+      <c r="I6" s="8"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="L6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="I7" s="8"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="L7" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" t="s">
         <v>83</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="5">
+      <c r="I8" s="8"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" t="s">
         <v>87</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="5">
+      <c r="I9" s="8"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="5" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="5">
+      <c r="I10" s="8"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" t="s">
         <v>95</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="5">
+      <c r="I11" s="8"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="5" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="5" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D12" t="s">
-        <v>324</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>35</v>
@@ -2193,25 +2324,27 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="5">
+      <c r="J12" s="6"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" t="s">
         <v>102</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>35</v>
@@ -2219,25 +2352,27 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="5">
+      <c r="J13" s="6"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="5" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="5" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" t="s">
         <v>106</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>108</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>35</v>
@@ -2245,25 +2380,27 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="5">
+      <c r="J14" s="6"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" t="s">
         <v>110</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>36</v>
@@ -2271,25 +2408,27 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="5">
+      <c r="J15" s="6"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="5" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" t="s">
         <v>114</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>36</v>
@@ -2297,36 +2436,39 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="5">
+      <c r="J16" s="6"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" t="s">
         <v>118</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="6"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="5">
+      <c r="K17" s="9"/>
+      <c r="L17" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
@@ -2337,79 +2479,82 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18"/>
       <c r="F18" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="J18" s="5">
+        <v>196</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="K18" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="L18" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E19"/>
       <c r="F19" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="I19" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="J19" s="5">
+        <v>197</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="K19" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="L19" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20"/>
       <c r="F20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="K20" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="L20" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="J20" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
@@ -2418,911 +2563,998 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" t="s">
         <v>173</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="L22" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="I21" s="10" t="s">
+      <c r="B23" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="L23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="L24" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="L26" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="K28" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="L30" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="L31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L32" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="L33" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K34" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="J21" s="5">
+      <c r="L34" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" t="s">
-        <v>172</v>
-      </c>
-      <c r="D22" t="s">
-        <v>174</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="J22" s="5">
+    <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="L35" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D23" t="s">
-        <v>175</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="I23" s="8" t="s">
+    <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" t="s">
+        <v>184</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="L36" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="L37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" t="s">
+        <v>186</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="L38" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" t="s">
+        <v>187</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="L39" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" t="s">
+        <v>188</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="J40" t="s">
+        <v>342</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="L40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" t="s">
+        <v>189</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="L41" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" t="s">
+        <v>255</v>
+      </c>
+      <c r="D42" t="s">
+        <v>264</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="K42" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="L42" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" t="s">
+        <v>256</v>
+      </c>
+      <c r="D43" t="s">
+        <v>265</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="K43" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="L43" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C44" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" t="s">
+        <v>266</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="J44" t="s">
+        <v>353</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="L44" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C45" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" t="s">
+        <v>267</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="K45" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="L45" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C46" t="s">
+        <v>259</v>
+      </c>
+      <c r="D46" t="s">
+        <v>268</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="K46" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="L46" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" t="s">
+        <v>190</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="J47" t="s">
+        <v>348</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="L47" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" t="s">
+        <v>191</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="J48" t="s">
+        <v>344</v>
+      </c>
+      <c r="K48" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="J23" s="5">
+      <c r="L48" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C49" t="s">
+        <v>269</v>
+      </c>
+      <c r="D49" t="s">
+        <v>270</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="L49" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C50" t="s">
+        <v>271</v>
+      </c>
+      <c r="D50" t="s">
+        <v>272</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="L50" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C51" t="s">
+        <v>273</v>
+      </c>
+      <c r="D51" t="s">
+        <v>274</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="J51" t="s">
+        <v>350</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="L51" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C52" t="s">
+        <v>275</v>
+      </c>
+      <c r="D52" t="s">
+        <v>282</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="K52" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="L52" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C53" t="s">
+        <v>276</v>
+      </c>
+      <c r="D53" t="s">
+        <v>281</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="K53" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="L53" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>277</v>
+      </c>
+      <c r="D54" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="K54" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="L54" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D55" t="s">
+        <v>279</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="K55" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="L55" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s">
+        <v>192</v>
+      </c>
+      <c r="L56" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C24" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="J24" s="5">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" t="s">
+        <v>193</v>
+      </c>
+      <c r="L57" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J25" s="5">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" t="s">
+        <v>150</v>
+      </c>
+      <c r="D58" t="s">
+        <v>194</v>
+      </c>
+      <c r="L58" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D59" t="s">
+        <v>252</v>
+      </c>
+      <c r="L59" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" t="s">
-        <v>178</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="J26" s="5">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D60" t="s">
+        <v>253</v>
+      </c>
+      <c r="L60" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="I27" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="I28" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" t="s">
-        <v>179</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="J30" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" t="s">
-        <v>166</v>
-      </c>
-      <c r="D31" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="J31" s="5">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="L61" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C32" t="s">
-        <v>165</v>
-      </c>
-      <c r="D32" t="s">
-        <v>181</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="J32" s="5">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="L62" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" t="s">
-        <v>182</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="J33" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C34" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" t="s">
-        <v>183</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="J34" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" t="s">
-        <v>184</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="J35" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" t="s">
-        <v>185</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="J36" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" t="s">
-        <v>186</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="J37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" t="s">
-        <v>187</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="J38" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C39" t="s">
-        <v>158</v>
-      </c>
-      <c r="D39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="J39" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C40" t="s">
-        <v>157</v>
-      </c>
-      <c r="D40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="J40" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" t="s">
-        <v>156</v>
-      </c>
-      <c r="D41" t="s">
-        <v>190</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="J41" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C42" t="s">
-        <v>257</v>
-      </c>
-      <c r="D42" t="s">
-        <v>266</v>
-      </c>
-      <c r="F42" s="6"/>
-      <c r="I42" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="J42" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C43" t="s">
-        <v>258</v>
-      </c>
-      <c r="D43" t="s">
-        <v>267</v>
-      </c>
-      <c r="F43" s="6"/>
-      <c r="I43" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="J43" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C44" t="s">
-        <v>259</v>
-      </c>
-      <c r="D44" t="s">
-        <v>268</v>
-      </c>
-      <c r="F44" s="6"/>
-      <c r="I44" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="J44" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C45" t="s">
-        <v>260</v>
-      </c>
-      <c r="D45" t="s">
-        <v>269</v>
-      </c>
-      <c r="F45" s="6"/>
-      <c r="I45" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="J45" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C46" t="s">
-        <v>261</v>
-      </c>
-      <c r="D46" t="s">
-        <v>270</v>
-      </c>
-      <c r="F46" s="6"/>
-      <c r="I46" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="J46" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" t="s">
-        <v>191</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="J47" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" t="s">
-        <v>154</v>
-      </c>
-      <c r="D48" t="s">
-        <v>192</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="J48" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C49" t="s">
-        <v>271</v>
-      </c>
-      <c r="D49" t="s">
-        <v>272</v>
-      </c>
-      <c r="F49" s="6"/>
-      <c r="I49" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="J49" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="C50" t="s">
-        <v>273</v>
-      </c>
-      <c r="D50" t="s">
-        <v>274</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="J50" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="C51" t="s">
-        <v>275</v>
-      </c>
-      <c r="D51" t="s">
-        <v>276</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="I51" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="J51" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C52" t="s">
-        <v>277</v>
-      </c>
-      <c r="D52" t="s">
-        <v>284</v>
-      </c>
-      <c r="F52" s="6"/>
-      <c r="I52" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="J52" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C53" t="s">
-        <v>278</v>
-      </c>
-      <c r="D53" t="s">
-        <v>283</v>
-      </c>
-      <c r="F53" s="6"/>
-      <c r="I53" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="J53" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C54" t="s">
-        <v>279</v>
-      </c>
-      <c r="D54" t="s">
-        <v>282</v>
-      </c>
-      <c r="F54" s="6"/>
-      <c r="I54" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="J54" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C55" t="s">
-        <v>280</v>
-      </c>
-      <c r="D55" t="s">
-        <v>281</v>
-      </c>
-      <c r="F55" s="6"/>
-      <c r="I55" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="J55" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C56" t="s">
-        <v>153</v>
-      </c>
-      <c r="D56" t="s">
-        <v>193</v>
-      </c>
-      <c r="J56" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" t="s">
-        <v>194</v>
-      </c>
-      <c r="J57" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58" t="s">
-        <v>151</v>
-      </c>
-      <c r="D58" t="s">
-        <v>195</v>
-      </c>
-      <c r="J58" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="D59" t="s">
-        <v>254</v>
-      </c>
-      <c r="J59" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="D60" t="s">
-        <v>255</v>
-      </c>
-      <c r="J60" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="J61" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J62" s="5">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J49" r:id="rId1" xr:uid="{F4001A4E-147C-4DA1-B793-B80C3CDB6A5D}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>